<commit_message>
main.py has new clean code
</commit_message>
<xml_diff>
--- a/data/Scopes.xlsx
+++ b/data/Scopes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashut\co-perform\Git_repo\Nabers_calculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F424373-C47C-453E-98E4-9B12AB9F6E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C5E87B-B5ED-465F-BA87-6EA9E5294068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9E97959-0B08-45DE-9CAD-8999FC1ED867}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{D9E97959-0B08-45DE-9CAD-8999FC1ED867}"/>
   </bookViews>
   <sheets>
     <sheet name="scope2_emissions" sheetId="1" r:id="rId1"/>
@@ -431,77 +431,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1731879F-E1BD-4BA2-A7F2-33DE6E856A0B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1">
+        <v>2019</v>
+      </c>
+      <c r="C1">
+        <v>2020</v>
+      </c>
+      <c r="D1">
         <v>2021</v>
       </c>
-      <c r="C1">
+      <c r="E1">
         <v>2022</v>
       </c>
-      <c r="D1">
+      <c r="F1">
         <v>2023</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.81</v>
+      </c>
+      <c r="C2">
+        <v>0.81</v>
+      </c>
+      <c r="D2">
         <v>0.79</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.73</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.68</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
+        <v>1.02</v>
+      </c>
+      <c r="C3">
+        <v>0.98</v>
+      </c>
+      <c r="D3">
         <v>0.96</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>0.85</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.79</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
         <v>0.17</v>
       </c>
       <c r="D4">
+        <v>0.16</v>
+      </c>
+      <c r="E4">
+        <v>0.17</v>
+      </c>
+      <c r="F4">
         <v>0.12</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.15</v>
       </c>
     </row>
@@ -512,49 +538,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C5A04F-8E3F-4B14-91F3-5046560AD597}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1">
+        <v>2019</v>
+      </c>
+      <c r="C1">
+        <v>2020</v>
+      </c>
+      <c r="D1">
         <v>2021</v>
       </c>
-      <c r="C1">
+      <c r="E1">
         <v>2022</v>
       </c>
-      <c r="D1">
+      <c r="F1">
         <v>2023</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.09</v>
+      </c>
+      <c r="C2">
+        <v>0.09</v>
+      </c>
+      <c r="D2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.06</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.05</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.04</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -562,16 +600,22 @@
         <v>0.1</v>
       </c>
       <c r="C3">
+        <v>0.11</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -579,12 +623,18 @@
         <v>0.02</v>
       </c>
       <c r="C4">
+        <v>0.02</v>
+      </c>
+      <c r="D4">
+        <v>0.02</v>
+      </c>
+      <c r="E4">
         <v>0.01</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.03</v>
       </c>
     </row>
@@ -598,7 +648,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>